<commit_message>
modify, add: intro, method, software, sparsity, summary
Former-commit-id: d0672130a739495a321a5cd2c944234a56c0fa59
Former-commit-id: a02643588f00cc72b4d6a1206b20f0e8b4bafdad
</commit_message>
<xml_diff>
--- a/experiment/analysis/SIPLIB_instance_information.xlsx
+++ b/experiment/analysis/SIPLIB_instance_information.xlsx
@@ -5,21 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="instance size info" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="instance_sparsity_info" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="solution report" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="instance_sparsity_cardinality" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="instance_sparsity_cardinality_info" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="instance_sparsity_partially_numerical" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="instance_sparsity_general" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="229">
   <si>
     <r>
       <t xml:space="preserve">1</t>
@@ -614,6 +615,9 @@
     <t>#nonzero</t>
   </si>
   <si>
+    <t>Density [0,1]</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1</t>
     </r>
@@ -638,6 +642,9 @@
     </r>
   </si>
   <si>
+    <t>1 / RT</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">2</t>
     </r>
@@ -662,13 +669,199 @@
     </r>
   </si>
   <si>
+    <t>(1+R)T</t>
+  </si>
+  <si>
+    <t>(1+2R) / (R+N)(1+R)T</t>
+  </si>
+  <si>
     <t>Complicating ©</t>
   </si>
   <si>
+    <t>(1+T)S / 4(R+N)</t>
+  </si>
+  <si>
     <t>DCLP</t>
   </si>
   <si>
+    <t>DCLP_</t>
+  </si>
+  <si>
     <t>SUC</t>
+  </si>
+  <si>
+    <t>SUC_D_S</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>\texttt{DCAP}</t>
+  </si>
+  <si>
+    <t>DCAP\_R\_T\_N\_S</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> stage (W)</t>
+    </r>
+  </si>
+  <si>
+    <t>(1+2R) / T(R+N)(1+R)</t>
+  </si>
+  <si>
+    <t>Complicating (T)</t>
+  </si>
+  <si>
+    <t>0.5T(T+1)</t>
+  </si>
+  <si>
+    <t>(1+T) / 4T(R+N)</t>
+  </si>
+  <si>
+    <t>DCLP\_</t>
+  </si>
+  <si>
+    <t>\texttt{MPTSPs}</t>
+  </si>
+  <si>
+    <t>MPTSPs\_D\_N\_S</t>
+  </si>
+  <si>
+    <t>N(N+1)</t>
+  </si>
+  <si>
+    <t>2N(N-1)</t>
+  </si>
+  <si>
+    <t>2(3N-2)(N-1)</t>
+  </si>
+  <si>
+    <t>(3N-2) / (N+1)N^2</t>
+  </si>
+  <si>
+    <t>N(N-1)</t>
+  </si>
+  <si>
+    <t>KN(N-1)</t>
+  </si>
+  <si>
+    <t>1 / KN(N-1)</t>
+  </si>
+  <si>
+    <t>3N(N-1)</t>
+  </si>
+  <si>
+    <t>3 / 2N(N-1)</t>
+  </si>
+  <si>
+    <t>\texttt{SIZES}</t>
+  </si>
+  <si>
+    <t>SIZES\_S</t>
+  </si>
+  <si>
+    <t>T(N+1)</t>
+  </si>
+  <si>
+    <t>2NT</t>
+  </si>
+  <si>
+    <t>3NT</t>
+  </si>
+  <si>
+    <t>3 / 2T(N+1)</t>
+  </si>
+  <si>
+    <t>0.5NT(T+1)(N+1)</t>
+  </si>
+  <si>
+    <t>(T+1) / 4N</t>
+  </si>
+  <si>
+    <t>0.5NT(T+1)</t>
+  </si>
+  <si>
+    <t>(T+1) / 8NT</t>
+  </si>
+  <si>
+    <t>\texttt{SMKP}</t>
+  </si>
+  <si>
+    <t>SMKP\_I\_S</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>2I</t>
+  </si>
+  <si>
+    <t>2IJ</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>IK</t>
+  </si>
+  <si>
+    <t>\texttt{SSLP}</t>
+  </si>
+  <si>
+    <t>SSLP\_I\_J\_S</t>
+  </si>
+  <si>
+    <t>I+J</t>
+  </si>
+  <si>
+    <t>(1+I)J</t>
+  </si>
+  <si>
+    <t>(1+2I)J</t>
+  </si>
+  <si>
+    <t>(1+2I) / (I+J)(1+I)</t>
+  </si>
+  <si>
+    <t>1 / (1+J)</t>
+  </si>
+  <si>
+    <t>\texttt{SUC}</t>
+  </si>
+  <si>
+    <t>SUC\_D\_S</t>
+  </si>
+  <si>
+    <t>G_s (2T+1)</t>
+  </si>
+  <si>
+    <t>G_f +G+(2G_f +G+N+L+\mathcal{L}+\mathcal{I}+\mathcal{R}+\mathcal{W})T</t>
+  </si>
+  <si>
+    <t>2G_s (T+1)</t>
   </si>
 </sst>
 </file>
@@ -849,7 +1042,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -986,6 +1179,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1005,8 +1210,8 @@
   </sheetPr>
   <dimension ref="A1:ALU100"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -5674,8 +5879,8 @@
   </sheetPr>
   <dimension ref="A1:ALU16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -5929,8 +6134,8 @@
   </sheetPr>
   <dimension ref="A1:ALT101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -7154,8 +7359,8 @@
   </sheetPr>
   <dimension ref="A1:ALX9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7407,22 +7612,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="30" width="15.6938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="30" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="30" width="20.1428571428571"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0"/>
       <c r="D2" s="30" t="s">
         <v>129</v>
       </c>
@@ -7433,7 +7649,7 @@
         <v>166</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>18</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7444,17 +7660,53 @@
         <v>156</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>168</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7464,23 +7716,23 @@
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7493,20 +7745,20 @@
         <v>39</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7519,20 +7771,20 @@
         <v>64</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7545,20 +7797,20 @@
         <v>70</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7566,25 +7818,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>156</v>
+      <c r="B23" s="32" t="s">
+        <v>165</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="32"/>
       <c r="C24" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7594,27 +7847,477 @@
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="14.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="15.6938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="64.4642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="15.1836734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="30" width="20.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="30" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="35"/>
+      <c r="C3" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="35"/>
+      <c r="C4" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="35"/>
+      <c r="C5" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="35"/>
+      <c r="C7" s="30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="35"/>
+      <c r="C8" s="30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="35"/>
+      <c r="C9" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="35"/>
+      <c r="C11" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="35"/>
+      <c r="C12" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="35"/>
+      <c r="C13" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="35"/>
+      <c r="C15" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="35"/>
+      <c r="C16" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="35"/>
+      <c r="C17" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="G18" s="30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="35"/>
+      <c r="C19" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="G19" s="30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="35"/>
+      <c r="C20" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="30" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="35"/>
+      <c r="C21" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="G22" s="35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="35"/>
+      <c r="C24" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="35"/>
+      <c r="C25" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="30" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>